<commit_message>
New plot for article
</commit_message>
<xml_diff>
--- a/migforecasting/underground/for article.xlsx
+++ b/migforecasting/underground/for article.xlsx
@@ -60,16 +60,20 @@
     <t>MSE</t>
   </si>
   <si>
-    <t>Big cities (test)</t>
+    <t>Big settlements</t>
   </si>
   <si>
-    <t>Small cities (test)</t>
+    <t>Small settlements</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0E+00"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -117,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -138,7 +142,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -154,6 +161,2796 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="0"/>
+              <a:t>MAE</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Аркуш1!$H$65</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MAE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Аркуш1!$G$66:$G$67</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Big settlements</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Small settlements</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Аркуш1!$H$66:$H$67</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1243.4855411336976</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>665.15273994932681</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0658-4E26-912C-49101F10C987}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="444"/>
+        <c:overlap val="-90"/>
+        <c:axId val="1765907824"/>
+        <c:axId val="1765908240"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1765907824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1765908240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1765908240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1765907824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="0"/>
+              <a:t>MSE</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Аркуш1!$J$65</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MSE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Аркуш1!$G$66:$G$67</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Big settlements</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Small settlements</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Аркуш1!$J$66:$J$67</c:f>
+              <c:numCache>
+                <c:formatCode>0.0E+00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>6.3054894442772114E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.494350600604522E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8744-435C-9400-5D0102D754D7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="444"/>
+        <c:overlap val="-90"/>
+        <c:axId val="1765907824"/>
+        <c:axId val="1765908240"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1765907824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1765908240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1765908240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.0E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1765907824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="0"/>
+              <a:t>MAPE</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Аркуш1!$I$65</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MAPE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Аркуш1!$G$66:$G$67</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Big settlements</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Small settlements</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Аркуш1!$I$66:$I$67</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3.0857253755454774</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.004877967075954</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A40C-482C-AB2F-BF56931263B7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="444"/>
+        <c:overlap val="-90"/>
+        <c:axId val="1765907824"/>
+        <c:axId val="1765908240"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1765907824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1765908240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1765908240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1765907824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="202">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="202">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="202">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>133352</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>914398</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Диаграмма 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>904875</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>361948</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Диаграмма 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -421,8 +3218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E4:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="V60" sqref="V60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2170,7 +4967,7 @@
       <c r="G66" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H66" s="7">
+      <c r="H66" s="9">
         <v>1243.4855411336976</v>
       </c>
       <c r="I66" s="7">
@@ -2187,7 +4984,7 @@
       <c r="G67" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H67" s="7">
+      <c r="H67" s="9">
         <v>665.15273994932681</v>
       </c>
       <c r="I67" s="7">
@@ -2203,5 +5000,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>